<commit_message>
refactor text matchers into own classes
</commit_message>
<xml_diff>
--- a/source/Vita.Predictor/SpreadSheets/keywords.xlsx
+++ b/source/Vita.Predictor/SpreadSheets/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\vita\source\Vita.Predictor\TextClassifiers\SpreadSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\vita\source\Vita.Predictor\SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13ACADCB-A172-4C02-A3D0-35EDACD4BB3B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F9FFBB-25D3-4470-A67E-D87C142CC4B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="948" firstSheet="1" activeTab="3" xr2:uid="{FCF0BCC7-E07F-42CD-B0A6-8479CEAB5437}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" tabRatio="948" activeTab="4" xr2:uid="{FCF0BCC7-E07F-42CD-B0A6-8479CEAB5437}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -18835,8 +18835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5A0D4B-DF32-4C07-BF05-7863F0FE63ED}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -19503,8 +19503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED92B709-C98F-4D84-A0C7-BF679CC19CF4}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>